<commit_message>
Labels indesign and expenses spreadsheet
</commit_message>
<xml_diff>
--- a/planning/space_management.xlsx
+++ b/planning/space_management.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christophe_rouleau-desrochers/Library/Mobile Documents/com~apple~CloudDocs/UBC/fuelinex/planning/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christophe_rouleau-desrochers/Documents/github/fuelinex/planning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BA4AD419-E7C9-F34A-A147-3C7AC8AA5689}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBE6184B-D527-F142-85D6-4C2B6A5B8283}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="1140" windowWidth="27640" windowHeight="16860" xr2:uid="{7E6AD438-2B84-C544-AE7D-1D05F851FA4F}"/>
+    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" xr2:uid="{7E6AD438-2B84-C544-AE7D-1D05F851FA4F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -181,9 +181,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -221,7 +221,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -327,7 +327,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -469,7 +469,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -479,13 +479,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF25ADC9-F134-804A-B28A-A6B3FBB83E9D}">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" zoomScale="162" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -496,7 +496,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -507,7 +507,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -518,7 +518,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -529,7 +529,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -540,7 +540,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -551,7 +551,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -562,7 +562,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -573,7 +573,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -584,7 +584,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -595,7 +595,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -606,15 +606,19 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>14</v>
       </c>
       <c r="C15">
         <v>48</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="E15">
+        <f>SUM(B15:C20)</f>
+        <v>204</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -709,14 +713,14 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C27">
         <v>15</v>
       </c>
       <c r="D27">
         <f t="shared" si="0"/>
-        <v>105</v>
+        <v>135</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
@@ -724,14 +728,14 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C28">
         <v>15</v>
       </c>
       <c r="D28">
         <f t="shared" si="0"/>
-        <v>105</v>
+        <v>135</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
@@ -754,14 +758,14 @@
         <v>25</v>
       </c>
       <c r="B31">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C31">
         <v>15</v>
       </c>
       <c r="D31">
         <f t="shared" si="0"/>
-        <v>105</v>
+        <v>135</v>
       </c>
     </row>
     <row r="33" spans="4:5" x14ac:dyDescent="0.2">
@@ -770,7 +774,7 @@
       </c>
       <c r="E33">
         <f>SUM(D25:D31)</f>
-        <v>315</v>
+        <v>405</v>
       </c>
     </row>
   </sheetData>

</xml_diff>